<commit_message>
Added data definition for 1st and 2nd
</commit_message>
<xml_diff>
--- a/Dataset Dictionary.xlsx
+++ b/Dataset Dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Assignments\Machine Learning\OilPricePrediction-TimeSeries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A6835A0-1BEE-4A99-845C-E540440CF5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE73B9E-DAE3-4E74-A882-D4F2A0DC78C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6C0381D5-8427-4994-971C-691892E8BDB3}"/>
   </bookViews>
@@ -36,22 +36,145 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Data Dictionary</t>
   </si>
   <si>
-    <t>Table Number</t>
-  </si>
-  <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Possible Data Analysis</t>
+  </si>
+  <si>
+    <t>This table could be used to see how a countries GDP, and poulation affects it's total export. Ultimately how will that affect the over all crude price. A major country should have significance on pricing.</t>
+  </si>
+  <si>
+    <t>Table 1.1: OPEC Members' facts and figures</t>
+  </si>
+  <si>
+    <t>Table 1.2: OPEC Members' crude oil production allocations</t>
+  </si>
+  <si>
+    <t>Table# and Name</t>
+  </si>
+  <si>
+    <t>This table contains geographical and export data of 13 OPEC Contries. Data like population, GDP, total export, natural gas export, crude oil export. Units are usally  barrels per day (b/d) and in million usd. Also, from the data it's a conclusion that among OPEC countries UAE and Saudi Arabia</t>
+  </si>
+  <si>
+    <t>This table contains how much each opec country was assigned to produce oil. For ex; UAE was assigned to produce 200 thousand barrels in a month. Some smaller countries weren't given a target/allocation and are represented by '-' in table. This could be considered as missing values. The granuality of this dataset varies a lot. For more recent year like 22, 21 it's a month, but for older years like 2005 it's a about a year.</t>
+  </si>
+  <si>
+    <t>Doesn’t tell much but just about the target. We could see if each country was able to match their target. And if a country missed it's target what was the impact of it in overall price.</t>
+  </si>
+  <si>
+    <t>Table 2.1: OPEC Members' population (million people)</t>
+  </si>
+  <si>
+    <t>This table again contains the population of each opec country and how it increaed over the years.</t>
+  </si>
+  <si>
+    <t>Doesn't help much in data analysis.</t>
+  </si>
+  <si>
+    <t>Summary 1</t>
+  </si>
+  <si>
+    <t>Macro-economics 2</t>
+  </si>
+  <si>
+    <t>Table 2.2: OPEC Members' Nominal GDP (at current market prices) (m $)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains OPEC memebers nominal GDP over the years. </t>
+  </si>
+  <si>
+    <t>Doesn't help either. Maybe we could see if nominal GDP is corelating with the price?</t>
+  </si>
+  <si>
+    <t>Table 2.3: OPEC Members real GDP growth rates (PPP based weights) (%)</t>
+  </si>
+  <si>
+    <t>Contains hwo the GDP has grown over the years. Since these are relative values to previous years, they are in negative reflecting the GDP has shrunk.</t>
+  </si>
+  <si>
+    <t>Same as above</t>
+  </si>
+  <si>
+    <t>Table 2.4: OPEC Members' values of exports of goods and services (m $)</t>
+  </si>
+  <si>
+    <t>Total exports of OPEC contries (including oil, natural gas, gold, and everything else)</t>
+  </si>
+  <si>
+    <t>Could be a useful feature</t>
+  </si>
+  <si>
+    <t>Table 2.5: OPEC Members' values of petroleum exports (m $)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total petroleum export. Some of them are missing values. The data is from 1960 to 2022 with a granulaity of a year. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>potential</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> feature</t>
+    </r>
+  </si>
+  <si>
+    <t>Table 2.6: OPEC Members' values of imports of goods and services(m $)</t>
+  </si>
+  <si>
+    <t>Total imports of goods and services. Same granuality as above.</t>
+  </si>
+  <si>
+    <t>Not so useful I think. As their import shouldn't affect much to oil prices.</t>
+  </si>
+  <si>
+    <t>Table 2.7: Current account balances in OPEC Members (m $)</t>
+  </si>
+  <si>
+    <t>What is current account Balance?  According to GPT: It is a broad measure that includes the trade balance (exports minus imports of goods and services), net income (such as interest and dividends) from abroad, and net current transfers (like foreign aid and remittances).
+When oil prices are high and exports are robust, the current account balance tends to show a surplus, as the revenue from oil exports exceeds the value of imported goods and services. Conversely, when oil prices are low or there are disruptions in oil exports, the current account balance may show a deficit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Could be a useful feature. As we can see a relational trend between this and price. Although usually price would get low, and the country would incur loss and then the account balance would reflect negative values. Still. </t>
+  </si>
+  <si>
+    <t>yet to add upstream data.</t>
+  </si>
+  <si>
+    <t>Oil data: Upstream 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +185,28 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
@@ -84,14 +229,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma 2" xfId="1" xr:uid="{EB78E461-4304-4FCF-9CF8-D19927E9193B}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -404,29 +562,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26698943-8ACC-43BC-B41B-849BBF6D83AF}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="82.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50.88671875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>